<commit_message>
League Table Update - Season Ender
</commit_message>
<xml_diff>
--- a/footy_stats_24_25.xlsx
+++ b/footy_stats_24_25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
   <si>
     <t>Matchday</t>
   </si>
@@ -299,6 +299,39 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Rich B, Rithwik, DB, Ash, Jarmaine, Hemansh</t>
+  </si>
+  <si>
+    <t>DC, Jordan, Chris, Gradwell, Matt Cook, Eduardo</t>
+  </si>
+  <si>
+    <t>7-6</t>
+  </si>
+  <si>
+    <t>Hemansh, DC</t>
+  </si>
+  <si>
+    <t>PJ, Rich B, Jarmaine, Gradwell, Eduardo, Rithwik</t>
+  </si>
+  <si>
+    <t>Matt Cook, Chris, DB, Harvey, Jack L, Tom</t>
+  </si>
+  <si>
+    <t>PJ, Matt Cook</t>
+  </si>
+  <si>
+    <t>JJ, PJ, Rich B, Harvey, Jack L</t>
+  </si>
+  <si>
+    <t>Ash, Matt Cook, DB, Gradwell, Rithwik</t>
+  </si>
+  <si>
+    <t>11-8</t>
+  </si>
+  <si>
+    <t>JJ, Ash</t>
   </si>
 </sst>
 </file>
@@ -590,6 +623,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="25.5"/>
+    <col customWidth="1" min="4" max="4" width="49.5"/>
     <col customWidth="1" min="7" max="7" width="20.63"/>
     <col customWidth="1" min="8" max="8" width="15.13"/>
   </cols>
@@ -1163,19 +1198,91 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="A21" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="8">
+        <v>45995.0</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22">
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="8">
+        <v>45694.0</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23">
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="A23" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="8">
+        <v>45701.0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24">
       <c r="C24" s="9"/>

</xml_diff>